<commit_message>
Started adding quandl as datasource
</commit_message>
<xml_diff>
--- a/data/meta_features.xlsx
+++ b/data/meta_features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0cap_2\MacroMan\SystematicMacro\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFAED11-5F9D-46E7-B23E-71933A6D379C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1018206-54F2-4282-8153-6AE485320297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6675" windowWidth="38640" windowHeight="15840" xr2:uid="{E4BEE590-548E-4391-B7C5-3A1E584A560D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{E4BEE590-548E-4391-B7C5-3A1E584A560D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="79">
   <si>
     <t>SOURCE</t>
   </si>
@@ -234,6 +234,45 @@
   </si>
   <si>
     <t>Copper_Price</t>
+  </si>
+  <si>
+    <t>RATEINF/CPI_USA</t>
+  </si>
+  <si>
+    <t>CPI_US</t>
+  </si>
+  <si>
+    <t>RATEINF/CPI_GBR</t>
+  </si>
+  <si>
+    <t>CPI_UK</t>
+  </si>
+  <si>
+    <t>RATEINF/CPI_ITA</t>
+  </si>
+  <si>
+    <t>CPI_IT</t>
+  </si>
+  <si>
+    <t>RATEINF/CPI_FRA</t>
+  </si>
+  <si>
+    <t>CPI_FR</t>
+  </si>
+  <si>
+    <t>RATEINF/CPI_EUR</t>
+  </si>
+  <si>
+    <t>RATEINF/CPI_DEU</t>
+  </si>
+  <si>
+    <t>CPI_EUR</t>
+  </si>
+  <si>
+    <t>CPI_GER</t>
+  </si>
+  <si>
+    <t>QUANDL</t>
   </si>
 </sst>
 </file>
@@ -596,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4D7372-E104-42F0-9C68-C06F66EB84FD}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1188,6 +1227,144 @@
         <v>60</v>
       </c>
     </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26">
+        <v>25</v>
+      </c>
+      <c r="G26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27">
+        <v>25</v>
+      </c>
+      <c r="G27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28">
+        <v>25</v>
+      </c>
+      <c r="G28" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29">
+        <v>25</v>
+      </c>
+      <c r="G29" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30">
+        <v>25</v>
+      </c>
+      <c r="G30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31">
+        <v>25</v>
+      </c>
+      <c r="G31" t="s">
+        <v>54</v>
+      </c>
+      <c r="H31" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Meta features and worked on data_loader to incorporate them into the model
</commit_message>
<xml_diff>
--- a/data/meta_features.xlsx
+++ b/data/meta_features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0cap_2\MacroMan\SystematicMacro\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1018206-54F2-4282-8153-6AE485320297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55FA956-34D9-43F8-8D3C-EFB7C9A38326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{E4BEE590-548E-4391-B7C5-3A1E584A560D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="93">
   <si>
     <t>SOURCE</t>
   </si>
@@ -273,6 +273,48 @@
   </si>
   <si>
     <t>QUANDL</t>
+  </si>
+  <si>
+    <t>ML/EMHYY</t>
+  </si>
+  <si>
+    <t>EM_HY_YIELD</t>
+  </si>
+  <si>
+    <t>ML/AAAEY</t>
+  </si>
+  <si>
+    <t>US_IG_YIELD</t>
+  </si>
+  <si>
+    <t>ML/BBBEY</t>
+  </si>
+  <si>
+    <t>US_CORP_YIELD</t>
+  </si>
+  <si>
+    <t>ML/EMCTRI</t>
+  </si>
+  <si>
+    <t>EM_CORP_RET</t>
+  </si>
+  <si>
+    <t>ML/USTRI</t>
+  </si>
+  <si>
+    <t>US_HY_YIELD</t>
+  </si>
+  <si>
+    <t>ML/EMHGY</t>
+  </si>
+  <si>
+    <t>EM_IG_YIELD</t>
+  </si>
+  <si>
+    <t>ML/EMHG</t>
+  </si>
+  <si>
+    <t>EMEA_CORP_YIELD</t>
   </si>
 </sst>
 </file>
@@ -635,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4D7372-E104-42F0-9C68-C06F66EB84FD}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A38" sqref="A31:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1365,6 +1407,146 @@
         <v>60</v>
       </c>
     </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+      <c r="G32" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+      <c r="G33" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+      <c r="G35" t="s">
+        <v>54</v>
+      </c>
+      <c r="H35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G36" t="s">
+        <v>54</v>
+      </c>
+      <c r="H36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+      <c r="G37" t="s">
+        <v>54</v>
+      </c>
+      <c r="H37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="s">
+        <v>62</v>
+      </c>
+      <c r="G38" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>